<commit_message>
Adiciona página de Análise Refugo com 4 quadrantes e gráfico de motivos
</commit_message>
<xml_diff>
--- a/3.1_DASH_MENSAL_01_26.xlsx
+++ b/3.1_DASH_MENSAL_01_26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xandy\Documents\GitHub\Dash_Mectrol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8644E390-B340-4D93-8A63-7C400CADE494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CD57F6-6F36-4B72-878E-0D3D13858EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="661" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13511,9 +13511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI305"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H120" sqref="H120"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R3" sqref="R3:AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37129,7 +37129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG55"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="V1" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="AG3" sqref="AG3"/>

</xml_diff>